<commit_message>
Added update cell value
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>No</t>
   </si>
@@ -96,6 +96,33 @@
   </si>
   <si>
     <t>Jez Humble</t>
+  </si>
+  <si>
+    <t>El que se duerme pierde</t>
+  </si>
+  <si>
+    <t>Tom Peter</t>
+  </si>
+  <si>
+    <t>Sin lugar a duda</t>
+  </si>
+  <si>
+    <t>Ana Gutierrez</t>
+  </si>
+  <si>
+    <t>El arte de dormir</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Buscando a Nemo</t>
+  </si>
+  <si>
+    <t>Humble Po</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -422,8 +449,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -448,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -506,8 +533,8 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6">
-        <v>52</v>
+      <c r="D6" t="n">
+        <v>37090.0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -577,6 +604,62 @@
         <v>23</v>
       </c>
       <c r="D11" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="n">
         <v>41.0</v>
       </c>
     </row>

</xml_diff>